<commit_message>
add bbl parameterization to HR4 and VHR4
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-hr4/cmip6_cmcc_cmcc-cm2-hr4_ocean.xlsx
+++ b/cmip6/models/cmcc-cm2-hr4/cmip6_cmcc_cmcc-cm2-hr4_ocean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/es-doc.cmcc/cmip6/models/cmcc-cm2-hr4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B24275-F062-6946-A8E2-5D9CCA4719D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C635B04-EB6C-7043-8425-66FBB4B1DA61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="3640" windowWidth="35000" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10940" yWindow="3640" windowWidth="35000" windowHeight="14180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="856">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -3915,7 +3915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -8342,8 +8342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8561,7 +8561,9 @@
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>711</v>
+      </c>
       <c r="AA36" s="6" t="s">
         <v>711</v>
       </c>
@@ -8592,7 +8594,9 @@
       </c>
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="11"/>
+      <c r="B40" s="11">
+        <v>1000</v>
+      </c>
     </row>
     <row r="42" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">

</xml_diff>